<commit_message>
Actualization of the Traceability Matrix, were added corrections
</commit_message>
<xml_diff>
--- a/Doc/Window lifter Docs/V-Cycle Process/V_Cycle Process Script.xlsx
+++ b/Doc/Window lifter Docs/V-Cycle Process/V_Cycle Process Script.xlsx
@@ -19,7 +19,7 @@
     <sheet name="Module Verification" sheetId="4" r:id="rId5"/>
     <sheet name="SW Validation" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -2006,7 +2006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Drafting of the chapter 1, 2, 3 in Design Specification window lifter
</commit_message>
<xml_diff>
--- a/Doc/Window lifter Docs/V-Cycle Process/V_Cycle Process Script.xlsx
+++ b/Doc/Window lifter Docs/V-Cycle Process/V_Cycle Process Script.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\AEP\drive AEP\Mod2 - Ing. de SW\V-Cycle Process\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="7890" yWindow="3180" windowWidth="15015" windowHeight="9330" activeTab="1"/>
   </bookViews>
@@ -19,7 +14,7 @@
     <sheet name="Module Verification" sheetId="4" r:id="rId5"/>
     <sheet name="SW Validation" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -152,9 +147,6 @@
     <t>Fix all defects found</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Design especification Document Template </t>
-  </si>
-  <si>
     <t>Document the Conceptual desing into the Design Especification Document</t>
   </si>
   <si>
@@ -321,13 +313,16 @@
   </si>
   <si>
     <t xml:space="preserve"> -  Checked in all working  documents into the repository </t>
+  </si>
+  <si>
+    <t>Design especification window lifter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,7 +535,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1654,7 +1649,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Right Arrow 2">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -1704,7 +1699,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1746,7 +1741,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1778,10 +1773,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1813,7 +1807,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1989,12 +1982,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2003,29 +1996,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.140625" customWidth="1"/>
     <col min="5" max="5" width="84.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5">
       <c r="C2" s="1"/>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5">
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5">
       <c r="C5" s="6" t="s">
         <v>0</v>
       </c>
@@ -2033,7 +2026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5" ht="18" customHeight="1">
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
@@ -2041,25 +2034,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="3:5" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" s="13" customFormat="1" ht="18" customHeight="1">
       <c r="C9" s="14"/>
       <c r="D9" s="40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="3:5" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" s="19" customFormat="1" ht="18" customHeight="1">
       <c r="C10" s="20"/>
       <c r="D10" s="41" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5">
       <c r="C11" s="5"/>
       <c r="D11" s="42" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:5">
       <c r="C13" s="10" t="s">
         <v>1</v>
       </c>
@@ -2070,7 +2063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:5">
       <c r="C14" s="51">
         <v>1</v>
       </c>
@@ -2081,28 +2074,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:5">
       <c r="C15" s="51"/>
       <c r="D15" s="52"/>
       <c r="E15" s="29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:5">
       <c r="C16" s="51"/>
       <c r="D16" s="52"/>
       <c r="E16" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5">
       <c r="C17" s="51"/>
       <c r="D17" s="52"/>
       <c r="E17" s="31" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5">
       <c r="C18" s="51">
         <v>2</v>
       </c>
@@ -2113,33 +2106,33 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="3:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5" s="21" customFormat="1">
       <c r="C19" s="51"/>
       <c r="D19" s="52"/>
       <c r="E19" s="29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5">
       <c r="C20" s="51"/>
       <c r="D20" s="52"/>
       <c r="E20" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:5">
       <c r="C21" s="51"/>
       <c r="D21" s="52"/>
       <c r="E21" s="29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:5">
       <c r="C22" s="51"/>
       <c r="D22" s="52"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:5">
       <c r="C23" s="51">
         <v>3</v>
       </c>
@@ -2150,60 +2143,60 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:5">
       <c r="C24" s="51"/>
       <c r="D24" s="52"/>
       <c r="E24" s="35" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5">
       <c r="C25" s="51"/>
       <c r="D25" s="52"/>
       <c r="E25" s="29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5">
       <c r="C26" s="51"/>
       <c r="D26" s="52"/>
       <c r="E26" s="26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:5" ht="30">
       <c r="C28" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5">
       <c r="C29" s="17"/>
       <c r="D29" s="34" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="3:5" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" s="21" customFormat="1" ht="30">
       <c r="C30" s="36"/>
       <c r="D30" s="34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="3:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" s="21" customFormat="1">
       <c r="C31" s="36"/>
       <c r="D31" s="34" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5">
       <c r="C32" s="18"/>
       <c r="D32" s="26" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" s="21" customFormat="1">
       <c r="C33" s="49"/>
       <c r="D33" s="50"/>
     </row>
@@ -2218,8 +2211,8 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1"/>
-    <hyperlink ref="D10" r:id="rId2"/>
-    <hyperlink ref="D11" r:id="rId3"/>
+    <hyperlink ref="D11" r:id="rId2"/>
+    <hyperlink ref="D10" r:id="rId3" display="2.0 Design\Design especification window lifter.doc"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -2228,35 +2221,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:E27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.7109375" customWidth="1"/>
     <col min="5" max="5" width="84.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5">
       <c r="C2" s="1"/>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5">
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5" ht="36" customHeight="1">
       <c r="C5" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="32.25" customHeight="1">
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
@@ -2264,31 +2257,31 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="3:5" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="C9" s="33"/>
       <c r="D9" s="29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="3:5" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="C10" s="33"/>
       <c r="D10" s="40" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" s="21" customFormat="1" ht="15.75" customHeight="1">
       <c r="C11" s="33"/>
       <c r="D11" s="40" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5">
       <c r="C12" s="5"/>
       <c r="D12" s="46" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5">
       <c r="C14" s="10" t="s">
         <v>1</v>
       </c>
@@ -2299,7 +2292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:5">
       <c r="C15" s="51">
         <v>1</v>
       </c>
@@ -2310,79 +2303,79 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:5">
       <c r="C16" s="51"/>
       <c r="D16" s="52"/>
       <c r="E16" s="29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5">
       <c r="C17" s="51"/>
       <c r="D17" s="52"/>
       <c r="E17" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5">
       <c r="C18" s="51"/>
       <c r="D18" s="52"/>
       <c r="E18" s="26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5">
       <c r="C19" s="51">
         <v>2</v>
       </c>
       <c r="D19" s="52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5">
       <c r="C20" s="51"/>
       <c r="D20" s="52"/>
       <c r="E20" s="30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5">
       <c r="C21" s="51"/>
       <c r="D21" s="52"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:5">
       <c r="C22" s="51"/>
       <c r="D22" s="52"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:5">
       <c r="C24" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5">
       <c r="C25" s="11"/>
       <c r="D25" s="30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" s="21" customFormat="1">
       <c r="C26" s="33"/>
       <c r="D26" s="30" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" s="21" customFormat="1">
       <c r="C27" s="5"/>
       <c r="D27" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2403,12 +2396,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:E31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="21"/>
     <col min="3" max="3" width="22.28515625" style="21" bestFit="1" customWidth="1"/>
@@ -2417,55 +2410,55 @@
     <col min="6" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5">
       <c r="C2" s="22"/>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5">
       <c r="C4" s="23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" ht="36" customHeight="1">
       <c r="C5" s="27" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="16.5" customHeight="1">
       <c r="C8" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="3:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" ht="16.5" customHeight="1">
       <c r="C9" s="33"/>
       <c r="D9" s="40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" ht="15.75" customHeight="1">
       <c r="C10" s="33"/>
       <c r="D10" s="40" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="15.75" customHeight="1">
       <c r="C11" s="33"/>
       <c r="D11" s="40" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5">
       <c r="C12" s="26"/>
       <c r="D12" s="46" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:5">
       <c r="C14" s="32" t="s">
         <v>1</v>
       </c>
@@ -2476,7 +2469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:5">
       <c r="C15" s="51">
         <v>1</v>
       </c>
@@ -2484,29 +2477,29 @@
         <v>34</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5">
       <c r="C16" s="51"/>
       <c r="D16" s="52"/>
       <c r="E16" s="29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5">
       <c r="C17" s="51"/>
       <c r="D17" s="52"/>
       <c r="E17" s="30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5">
       <c r="C18" s="51"/>
       <c r="D18" s="52"/>
       <c r="E18" s="31"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5">
       <c r="C19" s="51">
         <v>2</v>
       </c>
@@ -2517,26 +2510,26 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:5">
       <c r="C20" s="51"/>
       <c r="D20" s="52"/>
       <c r="E20" s="29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:5">
       <c r="C21" s="51"/>
       <c r="D21" s="52"/>
       <c r="E21" s="29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:5">
       <c r="C22" s="51"/>
       <c r="D22" s="52"/>
       <c r="E22" s="26"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:5">
       <c r="C23" s="51">
         <v>3</v>
       </c>
@@ -2547,49 +2540,49 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:5">
       <c r="C24" s="51"/>
       <c r="D24" s="52"/>
       <c r="E24" s="37" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:5">
       <c r="C25" s="51"/>
       <c r="D25" s="52"/>
       <c r="E25" s="29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:5">
       <c r="C26" s="51"/>
       <c r="D26" s="52"/>
       <c r="E26" s="26"/>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:5">
       <c r="C28" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5">
       <c r="C29" s="33"/>
       <c r="D29" s="34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5">
       <c r="C30" s="33"/>
       <c r="D30" s="34" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5">
       <c r="C31" s="26"/>
       <c r="D31" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2615,14 +2608,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:E25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="21"/>
     <col min="3" max="3" width="22.28515625" style="21" bestFit="1" customWidth="1"/>
@@ -2631,43 +2624,43 @@
     <col min="6" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5">
       <c r="C2" s="22"/>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5">
       <c r="C4" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" ht="36" customHeight="1">
       <c r="C5" s="27" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="19.5" customHeight="1">
       <c r="C8" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="48" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" ht="15.75" customHeight="1">
       <c r="C9" s="33"/>
       <c r="D9" s="29" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5">
       <c r="C10" s="26"/>
       <c r="D10" s="46" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:5">
       <c r="C12" s="32" t="s">
         <v>1</v>
       </c>
@@ -2678,90 +2671,90 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:5">
       <c r="C13" s="51">
         <v>1</v>
       </c>
       <c r="D13" s="52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5">
       <c r="C14" s="51"/>
       <c r="D14" s="52"/>
       <c r="E14" s="45" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5">
       <c r="C15" s="51"/>
       <c r="D15" s="52"/>
       <c r="E15" s="30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5">
       <c r="C16" s="51"/>
       <c r="D16" s="52"/>
       <c r="E16" s="31"/>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5">
       <c r="C17" s="51">
         <v>2</v>
       </c>
       <c r="D17" s="52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5">
       <c r="C18" s="51"/>
       <c r="D18" s="52"/>
       <c r="E18" s="29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" ht="45">
       <c r="C19" s="51"/>
       <c r="D19" s="52"/>
       <c r="E19" s="44" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5">
       <c r="C20" s="51"/>
       <c r="D20" s="52"/>
       <c r="E20" s="31"/>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:5">
       <c r="C22" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5">
       <c r="C23" s="33"/>
       <c r="D23" s="29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5">
       <c r="C24" s="33"/>
       <c r="D24" s="29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5">
       <c r="C25" s="26"/>
       <c r="D25" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2782,14 +2775,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:E32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="21"/>
     <col min="3" max="3" width="22.28515625" style="21" bestFit="1" customWidth="1"/>
@@ -2798,43 +2791,43 @@
     <col min="6" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5">
       <c r="C2" s="22"/>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5">
       <c r="C4" s="23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" ht="36" customHeight="1">
       <c r="C5" s="27" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="19.5" customHeight="1">
       <c r="C8" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="48" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" ht="15.75" customHeight="1">
       <c r="C9" s="33"/>
       <c r="D9" s="29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5">
       <c r="C10" s="26"/>
       <c r="D10" s="46" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:5">
       <c r="C12" s="32" t="s">
         <v>1</v>
       </c>
@@ -2845,129 +2838,129 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:5">
       <c r="C13" s="51">
         <v>1</v>
       </c>
       <c r="D13" s="52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5">
       <c r="C14" s="51"/>
       <c r="D14" s="52"/>
       <c r="E14" s="45" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5">
       <c r="C15" s="51"/>
       <c r="D15" s="52"/>
       <c r="E15" s="30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5">
       <c r="C16" s="51"/>
       <c r="D16" s="52"/>
       <c r="E16" s="31"/>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5">
       <c r="C17" s="51">
         <v>2</v>
       </c>
       <c r="D17" s="52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5">
       <c r="C18" s="51"/>
       <c r="D18" s="52"/>
       <c r="E18" s="29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" ht="30">
       <c r="C19" s="51"/>
       <c r="D19" s="52"/>
       <c r="E19" s="44" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5">
       <c r="C20" s="51"/>
       <c r="D20" s="52"/>
       <c r="E20" s="31"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:5">
       <c r="C23" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5">
       <c r="C24" s="33"/>
       <c r="D24" s="29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5">
       <c r="C25" s="33"/>
       <c r="D25" s="29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5">
       <c r="C26" s="33"/>
       <c r="D26" s="29" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5">
       <c r="C27" s="26"/>
       <c r="D27" s="26" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5">
       <c r="D28" s="39"/>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:5">
       <c r="C29" s="53"/>
       <c r="D29" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E29" s="38" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5">
       <c r="C30" s="53"/>
       <c r="D30" s="52"/>
       <c r="E30" s="29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" ht="30">
       <c r="C31" s="53"/>
       <c r="D31" s="52"/>
       <c r="E31" s="44" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" ht="30">
       <c r="C32" s="53"/>
       <c r="D32" s="52"/>
       <c r="E32" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>